<commit_message>
updated everything registration.login related in /Master
</commit_message>
<xml_diff>
--- a/Validation Test Form.xlsx
+++ b/Validation Test Form.xlsx
@@ -2,21 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Box Sync\BCIT\COMP 1536\Project\Collaboration\VirtualTour\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky\Dropbox\BCIT CST\COMP 1536\VirtualTour\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
-  <si>
-    <t>FORM on page:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Field ID</t>
   </si>
@@ -59,14 +57,88 @@
   </si>
   <si>
     <t>Problems</t>
+  </si>
+  <si>
+    <t>FORM on page: Registration</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>RegExp(/^[a-z0-9]{6,10}(?!.{1,})$/)</t>
+  </si>
+  <si>
+    <t>6-10 characters a-z lowercase, 0-9 only: for simplicity</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>RegExp(/^[A-z0-9.]{1,}(?=@)/i)</t>
+  </si>
+  <si>
+    <t>RegExp(/@bcit.ca(?!.{1,})/);</t>
+  </si>
+  <si>
+    <t>RegExp(/@gmail.com(?!.{1,})/);</t>
+  </si>
+  <si>
+    <t>RegExp(/@my.bcit.ca(?!.{1,})/);</t>
+  </si>
+  <si>
+    <t>Searches anything.anything before the @, then searches for the allowed 3 domains as specified, with nothing allowed after .ca/.com</t>
+  </si>
+  <si>
+    <t>loginid</t>
+  </si>
+  <si>
+    <t>RegExp(/^[a-zA-Z0-9]{6,10}(?!.{1,})$/)</t>
+  </si>
+  <si>
+    <t>6-10 characters a-z any case, 0-9 only: for simplicity</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>cpassword</t>
+  </si>
+  <si>
+    <t>anything goes, only 10 in length</t>
+  </si>
+  <si>
+    <t>FORM on page: Login</t>
+  </si>
+  <si>
+    <t>10 is short, yeah whatever, we'll deal with security later - whenever you decide to teach us it (or anything)</t>
+  </si>
+  <si>
+    <t>10 chars and below</t>
+  </si>
+  <si>
+    <t>anything goes in password</t>
+  </si>
+  <si>
+    <t>FORM on page: Contact us</t>
+  </si>
+  <si>
+    <t>TEST DOCUMENTATION for FORM on page: Registration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -94,8 +166,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -379,42 +470,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -422,40 +640,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -471,40 +689,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated milestone, and validatioin test form.
</commit_message>
<xml_diff>
--- a/Validation Test Form.xlsx
+++ b/Validation Test Form.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky\Dropbox\BCIT CST\COMP 1536\VirtualTour\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akemi\Google Drive\BCIT\COMP 1536\project\VirtualTour\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" tabRatio="91" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
   <si>
     <t>Field ID</t>
   </si>
@@ -38,24 +37,12 @@
     <t>Explanation</t>
   </si>
   <si>
-    <t>TEST DOCUMENTATION for FORM on page:</t>
-  </si>
-  <si>
     <t>FIELD LEVEL TESTING</t>
   </si>
   <si>
-    <t>Problem</t>
-  </si>
-  <si>
-    <t>Improvements made</t>
-  </si>
-  <si>
     <t>FORM LEVEL TESTING</t>
   </si>
   <si>
-    <t>Form Flow</t>
-  </si>
-  <si>
     <t>Problems</t>
   </si>
   <si>
@@ -122,14 +109,201 @@
     <t>FORM on page: Contact us</t>
   </si>
   <si>
-    <t>TEST DOCUMENTATION for FORM on page: Registration</t>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Improvements Made</t>
+  </si>
+  <si>
+    <t>Log In</t>
+  </si>
+  <si>
+    <t>Log in page doesn't need username or password validation. Password does not show as asterisks.</t>
+  </si>
+  <si>
+    <t>Unable to cycle back to Username input by pressing Tab</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Able to input only '@bcit.ca'. Also able to input 'em@il@bcit.ca'.</t>
+  </si>
+  <si>
+    <t>need space between loginID</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>When submitting, prompts user to input e-mail, then refreshes page and clears the e-mail text box.</t>
+  </si>
+  <si>
+    <t>Can register without having to accept TOS.</t>
+  </si>
+  <si>
+    <t>Fixed.</t>
+  </si>
+  <si>
+    <t>Error given when password is more than 10 characters long, can put in empty string as password and still valid.</t>
+  </si>
+  <si>
+    <t>"usernameErrorField" and  "passErrorField"</t>
+  </si>
+  <si>
+    <t>"username"</t>
+  </si>
+  <si>
+    <t>"email"</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>"password"</t>
+  </si>
+  <si>
+    <t>"agreeErrorField"</t>
+  </si>
+  <si>
+    <t>"email" and "submit"</t>
+  </si>
+  <si>
+    <t>contactFieldValue == ""</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/@my.bcit.ca$/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/@gmail.com$/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contactEmailValue == ""</t>
+    </r>
+  </si>
+  <si>
+    <t>If the e-mail entered is not a bcit or a gmail, error "Please enter a valid email."</t>
+  </si>
+  <si>
+    <t>/[&amp;'"\$\\</t>
+  </si>
+  <si>
+    <t>username, subject, contact_Input</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>If any input has  &amp; ' " \ $, replace with appropriate symbols.</t>
+  </si>
+  <si>
+    <t>FORM on page: Contact Us</t>
+  </si>
+  <si>
+    <t>If nothing typed in section, error "please enter a valid input".</t>
+  </si>
+  <si>
+    <t>FORM on page: Log In</t>
+  </si>
+  <si>
+    <t>(/^[a-z0-9]{6,10}(?!.{1,})$/)</t>
+  </si>
+  <si>
+    <t>a-z, 0-9 includes - _ and . 6-10 characters total, after first match, no more. If it doesn't meet these parameters, "Username Invalid."</t>
+  </si>
+  <si>
+    <t>pass.length &gt; 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if password length more than 10, invalid. </t>
+  </si>
+  <si>
+    <t>FORM on page: Register</t>
+  </si>
+  <si>
+    <t>Added space between login and ID.</t>
+  </si>
+  <si>
+    <t>a-z, 0-9 includes - _ and . 6-10 characters total, after first match, no more. If it doesn't meet these requirements, "Please enter a valid username."</t>
+  </si>
+  <si>
+    <t>(/^[A-z0-9.]{1,}(?=@)/i), and (/@my.bcit.ca(?!.{1,})/), and (/@bcit.ca(?!.{1,})/);, and (/@gmail.com(?!.{1,})/)</t>
+  </si>
+  <si>
+    <t>e-mail must be bcit or gmail domain. If it doesn't meet requirements, "Email invalid."</t>
+  </si>
+  <si>
+    <t>(/^[a-zA-Z0-9]{6,10}(?!.{1,})$/)</t>
+  </si>
+  <si>
+    <t>a-z, A-Z, 0-9 :: 6-10 characters total, after first match, no more. If it doesn't meet requirements, "Please enter valid loginID."</t>
+  </si>
+  <si>
+    <t>true if length less than 10 and password===cpass. If it doesn't meet requirements, either "Passwords do not match", or "Password longer than 10."</t>
+  </si>
+  <si>
+    <t>pass.length &gt; 10 &amp;&amp; pass.length &lt;= 0 AND pass === confirmpass</t>
+  </si>
+  <si>
+    <t>!consentYes.checked</t>
+  </si>
+  <si>
+    <t>user must agree to TOS. If not, "Please agree to TOS."</t>
+  </si>
+  <si>
+    <t>consentYes, consentNo, agreeErrorField.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +313,31 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -166,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,6 +387,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -485,7 +690,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -503,81 +708,81 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -595,29 +800,29 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -638,98 +843,349 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>31</v>
-      </c>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="A1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final edits for milestone 4
</commit_message>
<xml_diff>
--- a/Validation Test Form.xlsx
+++ b/Validation Test Form.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Box Sync\BCIT\COMP 1536\Project\Collaboration\VirtualTour\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacky\Dropbox\BCIT CST\COMP 1536\VirtualTour\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="250" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" tabRatio="317" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -257,9 +258,6 @@
     <t>pass.length &gt; 10</t>
   </si>
   <si>
-    <t xml:space="preserve">if password length more than 10, invalid. </t>
-  </si>
-  <si>
     <t>FORM on page: Register</t>
   </si>
   <si>
@@ -309,12 +307,15 @@
   </si>
   <si>
     <t>Added space between login and ID</t>
+  </si>
+  <si>
+    <t>if password length more than 10, invalid - registration made it so</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -693,21 +694,21 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -718,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -729,7 +730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -740,28 +741,28 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -772,7 +773,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -783,7 +784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -792,14 +793,14 @@
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
@@ -810,7 +811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -821,7 +822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -832,7 +833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
@@ -857,24 +858,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="101.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="101.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -882,7 +883,7 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -896,7 +897,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -907,10 +908,10 @@
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -921,10 +922,10 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -935,10 +936,10 @@
         <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -949,10 +950,10 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -963,10 +964,10 @@
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>4</v>
       </c>
@@ -974,7 +975,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -988,7 +989,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -999,10 +1000,10 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1013,7 +1014,7 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1031,25 +1032,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="2" max="2" width="94.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1082,7 +1083,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -1093,14 +1094,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1122,7 +1123,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1130,17 +1131,17 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1159,51 +1160,51 @@
         <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
         <v>62</v>
       </c>
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
         <v>64</v>
       </c>
-      <c r="C16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
         <v>67</v>
       </c>
-      <c r="C17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>